<commit_message>
Hack in a way to make network objects MY way! (Cause the built in photon one is CRAP)
</commit_message>
<xml_diff>
--- a/Docs/40map.xlsx
+++ b/Docs/40map.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="1583" documentId="11_2F206C6948C74EE3E979BAFA89738C9863138395" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DA5D9A4A-9F89-4105-9AAB-F96320619BF9}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomle\git\Hong-Kong-three-six-tee\Docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8724BC8E-1032-4A27-BE34-ABF169B2E9D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16920" yWindow="0" windowWidth="11985" windowHeight="15585" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="地圖" sheetId="1" r:id="rId1"/>
@@ -19,8 +24,8 @@
     <sheet name="立法" sheetId="8" r:id="rId9"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">博彩!$B$1:$D$10</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">地點!$A$1:$F$41</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">博彩!$B$1:$D$10</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -40,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="312">
   <si>
     <t>竹篙灣隔離中心
 Quarantine Centre</t>
@@ -1022,6 +1027,18 @@
   </si>
   <si>
     <t>0.00017*運氣</t>
+  </si>
+  <si>
+    <t>Hold for Effects</t>
+  </si>
+  <si>
+    <t>Special Trigger</t>
+  </si>
+  <si>
+    <t>Place on tiles</t>
+  </si>
+  <si>
+    <t>Use on turn</t>
   </si>
 </sst>
 </file>
@@ -1032,21 +1049,21 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1058,28 +1075,28 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF70AD47"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFC65911"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1091,7 +1108,7 @@
     <font>
       <sz val="48"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1155,12 +1172,12 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="22">
+  <fills count="28">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1284,6 +1301,42 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1470,7 +1523,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1618,6 +1671,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1952,7 +2013,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CD18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BL1" workbookViewId="0">
+    <sheetView topLeftCell="BL1" workbookViewId="0">
       <selection activeCell="AQ5" sqref="AQ5"/>
     </sheetView>
   </sheetViews>
@@ -2970,14 +3031,15 @@
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E31" sqref="E31:E32"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9" style="37"/>
     <col min="2" max="2" width="11.5" style="56" customWidth="1"/>
-    <col min="3" max="5" width="9" style="37"/>
+    <col min="3" max="3" width="11.375" style="37" customWidth="1"/>
+    <col min="4" max="5" width="9" style="37"/>
     <col min="6" max="6" width="9" style="37" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9" style="37"/>
   </cols>
@@ -3747,10 +3809,10 @@
   <dimension ref="B2:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="3" max="3" width="63.125" customWidth="1"/>
   </cols>
@@ -3782,7 +3844,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="5" spans="2:4">
+    <row r="5" spans="2:4" ht="16.5">
       <c r="B5" t="s">
         <v>128</v>
       </c>
@@ -3820,7 +3882,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="9" spans="2:4">
+    <row r="9" spans="2:4" ht="16.5">
       <c r="B9" t="s">
         <v>138</v>
       </c>
@@ -3835,14 +3897,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C66F7F66-07BF-47F6-80DF-8CB7F4D949B6}">
-  <dimension ref="B1:J23"/>
+  <dimension ref="B1:J29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
+    <col min="2" max="2" width="16.75" customWidth="1"/>
+    <col min="3" max="3" width="16.125" customWidth="1"/>
     <col min="4" max="4" width="33.25" customWidth="1"/>
     <col min="5" max="5" width="20.875" customWidth="1"/>
     <col min="9" max="9" width="44.875" customWidth="1"/>
@@ -3872,7 +3936,7 @@
       </c>
     </row>
     <row r="2" spans="2:10">
-      <c r="B2" t="s">
+      <c r="B2" s="73" t="s">
         <v>147</v>
       </c>
       <c r="D2" t="s">
@@ -3889,7 +3953,7 @@
       </c>
     </row>
     <row r="3" spans="2:10">
-      <c r="B3" t="s">
+      <c r="B3" s="73" t="s">
         <v>151</v>
       </c>
       <c r="D3" t="s">
@@ -3906,7 +3970,7 @@
       </c>
     </row>
     <row r="4" spans="2:10">
-      <c r="B4" t="s">
+      <c r="B4" s="70" t="s">
         <v>153</v>
       </c>
       <c r="D4" t="s">
@@ -3920,7 +3984,7 @@
       </c>
     </row>
     <row r="5" spans="2:10">
-      <c r="B5" t="s">
+      <c r="B5" s="70" t="s">
         <v>156</v>
       </c>
       <c r="D5" t="s">
@@ -3933,8 +3997,8 @@
         <v>158</v>
       </c>
     </row>
-    <row r="6" spans="2:10">
-      <c r="B6" t="s">
+    <row r="6" spans="2:10" ht="16.5">
+      <c r="B6" s="70" t="s">
         <v>159</v>
       </c>
       <c r="D6" t="s">
@@ -3950,8 +4014,8 @@
         <v>161</v>
       </c>
     </row>
-    <row r="7" spans="2:10">
-      <c r="B7" t="s">
+    <row r="7" spans="2:10" ht="16.5">
+      <c r="B7" s="72" t="s">
         <v>162</v>
       </c>
       <c r="D7" t="s">
@@ -3971,7 +4035,7 @@
       </c>
     </row>
     <row r="8" spans="2:10">
-      <c r="B8" t="s">
+      <c r="B8" s="70" t="s">
         <v>166</v>
       </c>
       <c r="D8" t="s">
@@ -3984,8 +4048,8 @@
         <v>168</v>
       </c>
     </row>
-    <row r="9" spans="2:10">
-      <c r="B9" t="s">
+    <row r="9" spans="2:10" ht="16.5">
+      <c r="B9" s="70" t="s">
         <v>169</v>
       </c>
       <c r="D9" t="s">
@@ -4001,8 +4065,8 @@
         <v>171</v>
       </c>
     </row>
-    <row r="10" spans="2:10">
-      <c r="B10" t="s">
+    <row r="10" spans="2:10" ht="16.5">
+      <c r="B10" s="72" t="s">
         <v>172</v>
       </c>
       <c r="D10" t="s">
@@ -4015,22 +4079,22 @@
         <v>174</v>
       </c>
     </row>
-    <row r="11" spans="2:10">
-      <c r="B11" t="s">
+    <row r="11" spans="2:10" ht="16.5">
+      <c r="B11" s="70" t="s">
         <v>175</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="75" t="s">
         <v>176</v>
       </c>
       <c r="F11" s="57" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="2:10">
-      <c r="B12" t="s">
+    <row r="12" spans="2:10" ht="16.5">
+      <c r="B12" s="73" t="s">
         <v>177</v>
       </c>
-      <c r="D12" s="57" t="s">
+      <c r="D12" s="76" t="s">
         <v>178</v>
       </c>
       <c r="E12" t="s">
@@ -4043,66 +4107,66 @@
         <v>150</v>
       </c>
     </row>
-    <row r="13" spans="2:10">
-      <c r="B13" t="s">
+    <row r="13" spans="2:10" ht="16.5">
+      <c r="B13" s="70" t="s">
         <v>180</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="75" t="s">
         <v>181</v>
       </c>
       <c r="F13" s="57" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="2:10">
-      <c r="B14" t="s">
+    <row r="14" spans="2:10" ht="16.5">
+      <c r="B14" s="71" t="s">
         <v>182</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="75" t="s">
         <v>183</v>
       </c>
       <c r="F14" s="57" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="2:10">
-      <c r="B15" t="s">
+    <row r="15" spans="2:10" ht="16.5">
+      <c r="B15" s="70" t="s">
         <v>184</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="75" t="s">
         <v>185</v>
       </c>
       <c r="F15" s="57" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="2:10">
-      <c r="B16" t="s">
+    <row r="16" spans="2:10" ht="16.5">
+      <c r="B16" s="72" t="s">
         <v>186</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="75" t="s">
         <v>187</v>
       </c>
       <c r="F16" s="57" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="2:10">
-      <c r="B17" t="s">
+    <row r="17" spans="2:10" ht="16.5">
+      <c r="B17" s="73" t="s">
         <v>188</v>
       </c>
-      <c r="D17" s="57" t="s">
+      <c r="D17" s="76" t="s">
         <v>189</v>
       </c>
       <c r="F17" s="57" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="18" spans="2:10">
-      <c r="B18" t="s">
+    <row r="18" spans="2:10" ht="16.5">
+      <c r="B18" s="73" t="s">
         <v>190</v>
       </c>
-      <c r="D18" s="57" t="s">
+      <c r="D18" s="76" t="s">
         <v>191</v>
       </c>
       <c r="F18" s="57" t="s">
@@ -4112,11 +4176,11 @@
         <v>192</v>
       </c>
     </row>
-    <row r="19" spans="2:10">
-      <c r="B19" t="s">
+    <row r="19" spans="2:10" ht="16.5">
+      <c r="B19" s="70" t="s">
         <v>193</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="75" t="s">
         <v>194</v>
       </c>
       <c r="F19" s="57" t="s">
@@ -4126,11 +4190,11 @@
         <v>195</v>
       </c>
     </row>
-    <row r="20" spans="2:10">
-      <c r="B20" t="s">
+    <row r="20" spans="2:10" ht="16.5">
+      <c r="B20" s="71" t="s">
         <v>196</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="75" t="s">
         <v>197</v>
       </c>
       <c r="E20" t="s">
@@ -4140,11 +4204,11 @@
         <v>94</v>
       </c>
     </row>
-    <row r="21" spans="2:10">
-      <c r="B21" t="s">
+    <row r="21" spans="2:10" ht="16.5">
+      <c r="B21" s="73" t="s">
         <v>198</v>
       </c>
-      <c r="D21" s="57" t="s">
+      <c r="D21" s="76" t="s">
         <v>199</v>
       </c>
       <c r="F21" t="s">
@@ -4160,11 +4224,11 @@
         <v>201</v>
       </c>
     </row>
-    <row r="22" spans="2:10">
-      <c r="B22" s="57" t="s">
+    <row r="22" spans="2:10" ht="16.5">
+      <c r="B22" s="74" t="s">
         <v>202</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="75" t="s">
         <v>203</v>
       </c>
       <c r="F22" t="s">
@@ -4180,15 +4244,39 @@
         <v>201</v>
       </c>
     </row>
-    <row r="23" spans="2:10">
-      <c r="B23" t="s">
+    <row r="23" spans="2:10" ht="16.5">
+      <c r="B23" s="71" t="s">
         <v>204</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="75" t="s">
         <v>205</v>
       </c>
       <c r="F23" s="57" t="s">
         <v>114</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10">
+      <c r="B25" s="69"/>
+      <c r="C25" s="73"/>
+    </row>
+    <row r="26" spans="2:10">
+      <c r="B26" t="s">
+        <v>311</v>
+      </c>
+      <c r="C26" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10">
+      <c r="B28" s="71"/>
+      <c r="C28" s="72"/>
+    </row>
+    <row r="29" spans="2:10">
+      <c r="B29" t="s">
+        <v>309</v>
+      </c>
+      <c r="C29" t="s">
+        <v>310</v>
       </c>
     </row>
   </sheetData>
@@ -4214,7 +4302,7 @@
       <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="3" max="3" width="26.875" customWidth="1"/>
     <col min="4" max="4" width="44.75" customWidth="1"/>
@@ -4237,7 +4325,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="2" spans="2:9">
+    <row r="2" spans="2:9" ht="16.5">
       <c r="B2" s="51" t="s">
         <v>72</v>
       </c>
@@ -4251,7 +4339,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="3" spans="2:9">
+    <row r="3" spans="2:9" ht="16.5">
       <c r="B3" s="51" t="s">
         <v>72</v>
       </c>
@@ -4265,7 +4353,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="4" spans="2:9">
+    <row r="4" spans="2:9" ht="16.5">
       <c r="B4" s="51" t="s">
         <v>72</v>
       </c>
@@ -4279,7 +4367,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="5" spans="2:9">
+    <row r="5" spans="2:9" ht="16.5">
       <c r="B5" s="51" t="s">
         <v>72</v>
       </c>
@@ -4294,7 +4382,7 @@
       </c>
       <c r="I5" s="51"/>
     </row>
-    <row r="6" spans="2:9">
+    <row r="6" spans="2:9" ht="16.5">
       <c r="B6" s="51" t="s">
         <v>72</v>
       </c>
@@ -4324,7 +4412,7 @@
       </c>
       <c r="I7" s="51"/>
     </row>
-    <row r="8" spans="2:9">
+    <row r="8" spans="2:9" ht="16.5">
       <c r="B8" s="51" t="s">
         <v>72</v>
       </c>
@@ -4352,7 +4440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:9">
+    <row r="10" spans="2:9" ht="16.5">
       <c r="B10" s="51" t="s">
         <v>72</v>
       </c>
@@ -4380,7 +4468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:9">
+    <row r="12" spans="2:9" ht="16.5">
       <c r="B12" s="51" t="s">
         <v>74</v>
       </c>
@@ -4394,7 +4482,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="13" spans="2:9">
+    <row r="13" spans="2:9" ht="16.5">
       <c r="B13" s="51" t="s">
         <v>74</v>
       </c>
@@ -4408,7 +4496,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="14" spans="2:9">
+    <row r="14" spans="2:9" ht="16.5">
       <c r="B14" s="51" t="s">
         <v>74</v>
       </c>
@@ -4422,7 +4510,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="15" spans="2:9">
+    <row r="15" spans="2:9" ht="16.5">
       <c r="B15" s="51" t="s">
         <v>74</v>
       </c>
@@ -4436,7 +4524,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="16" spans="2:9">
+    <row r="16" spans="2:9" ht="16.5">
       <c r="B16" s="51" t="s">
         <v>74</v>
       </c>
@@ -4520,7 +4608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:6">
+    <row r="22" spans="2:6" ht="16.5">
       <c r="B22" s="51" t="s">
         <v>114</v>
       </c>
@@ -4534,7 +4622,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="23" spans="2:6">
+    <row r="23" spans="2:6" ht="16.5">
       <c r="B23" s="51" t="s">
         <v>114</v>
       </c>
@@ -4548,7 +4636,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="24" spans="2:6">
+    <row r="24" spans="2:6" ht="16.5">
       <c r="B24" s="51" t="s">
         <v>114</v>
       </c>
@@ -4562,7 +4650,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="25" spans="2:6">
+    <row r="25" spans="2:6" ht="16.5">
       <c r="B25" s="51" t="s">
         <v>114</v>
       </c>
@@ -4607,7 +4695,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:6">
+    <row r="28" spans="2:6" ht="16.5">
       <c r="B28" s="51" t="s">
         <v>114</v>
       </c>
@@ -4621,7 +4709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="2:6">
+    <row r="29" spans="2:6" ht="16.5">
       <c r="B29" s="51" t="s">
         <v>114</v>
       </c>
@@ -4635,7 +4723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:6">
+    <row r="30" spans="2:6" ht="16.5">
       <c r="B30" s="51" t="s">
         <v>114</v>
       </c>
@@ -4663,7 +4751,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:6">
+    <row r="32" spans="2:6" ht="16.5">
       <c r="B32" s="51" t="s">
         <v>119</v>
       </c>
@@ -4677,7 +4765,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="33" spans="2:6">
+    <row r="33" spans="2:6" ht="16.5">
       <c r="B33" s="51" t="s">
         <v>119</v>
       </c>
@@ -4691,7 +4779,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="34" spans="2:6">
+    <row r="34" spans="2:6" ht="16.5">
       <c r="B34" s="51" t="s">
         <v>119</v>
       </c>
@@ -4705,7 +4793,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="35" spans="2:6">
+    <row r="35" spans="2:6" ht="16.5">
       <c r="B35" s="51" t="s">
         <v>119</v>
       </c>
@@ -4792,7 +4880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="2:6">
+    <row r="41" spans="2:6" ht="16.5">
       <c r="B41" s="51" t="s">
         <v>119</v>
       </c>
@@ -4819,7 +4907,7 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="2:4">
       <c r="D1" t="s">
@@ -4848,7 +4936,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="4" spans="2:4">
+    <row r="4" spans="2:4" ht="16.5">
       <c r="B4" s="57" t="s">
         <v>202</v>
       </c>
@@ -4872,7 +4960,7 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="2" max="2" width="18" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
@@ -4886,7 +4974,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="2" spans="2:4">
+    <row r="2" spans="2:4" ht="16.5">
       <c r="B2" s="57" t="s">
         <v>290</v>
       </c>
@@ -4897,7 +4985,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="3" spans="2:4">
+    <row r="3" spans="2:4" ht="16.5">
       <c r="B3" s="57" t="s">
         <v>292</v>
       </c>
@@ -4996,7 +5084,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5008,7 +5096,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>